<commit_message>
Add Sync button functionality and fix routes for fines page
</commit_message>
<xml_diff>
--- a/scripts/violations_details.xlsx
+++ b/scripts/violations_details.xlsx
@@ -14,33 +14,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Details</t>
   </si>
   <si>
     <t>Pay now
-CADILLAC ESCALADE, 2023, Blue
-N
-85540
+NISSAN VERSA, 2024, Blue
+Q
+89764
 Date and Time of Issuing The Fine:
-14 Jul 2025, 12:10 am
+19 Jul 2025, 8:50 am
 Location:
-Ras Al khour St
+GPS Location
 Source:
 Dubai Police
 Amount:
-AED 600
+AED 500
 Payable Black Points:
 -
 Online declaration:
 NO
 Fine Number:
-7037866556
+9010811131
 Details:
-Exceeding maximum speed limit by not more than 30 km h
+Parking in a wrong way
 Dispute:
 Please contact Dubai Police for details about disputing your fine.</t>
+  </si>
+  <si>
+    <t>Pay now
+KIA PEGAS, 2024, White
+U
+87907
+Date and Time of Issuing The Fine:
+16 Jul 2025, 7:55 pm
+Location:
+-
+Source:
+RTA (Parking Fines)
+Amount:
+AED 100
+Payable Black Points:
+-
+Online declaration:
+NO
+Fine Number:
+24067325
+Details:
+Parking Fine
+Dispute:
+Click here to apply for a request to dispute this fine.</t>
   </si>
   <si>
     <t>Pay now
@@ -422,7 +446,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -443,6 +467,11 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix CSRF token issue for sync button - add CSRF token to Inertia shared props
</commit_message>
<xml_diff>
--- a/scripts/violations_details.xlsx
+++ b/scripts/violations_details.xlsx
@@ -14,9 +14,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Details</t>
+  </si>
+  <si>
+    <t>Pay now
+RANGE ROVER SPORT, 2023, Golden
+BB
+90835
+Date and Time of Issuing The Fine:
+19 Jul 2025, 1:24 pm
+Location:
+-
+Source:
+RTA (Parking Fines)
+Amount:
+AED 150
+Payable Black Points:
+-
+Online declaration:
+NO
+Fine Number:
+24059326
+Details:
+Parking Fine
+Dispute:
+Click here to apply for a request to dispute this fine.</t>
   </si>
   <si>
     <t>Pay now
@@ -446,7 +470,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -472,6 +496,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>